<commit_message>
Adding Leah Blechschmidt Malus domestica Canada 18-19
</commit_message>
<xml_diff>
--- a/Final_Data/Supporting_files/Verified_studies/FINAL_Data ownership.xlsx
+++ b/Final_Data/Supporting_files/Verified_studies/FINAL_Data ownership.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8278" uniqueCount="749">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8306" uniqueCount="754">
   <si>
     <t xml:space="preserve">study_id</t>
   </si>
@@ -2225,9 +2225,6 @@
     <t xml:space="preserve">Diego N. Nabaes Jodar</t>
   </si>
   <si>
-    <t xml:space="preserve">Universidad Nacional de Rio Negro, Instituto de Investigaciones en Recursos Naturales, Agroecologia y Desarrollo Rural, Rio Negro, Argentina</t>
-  </si>
-  <si>
     <t xml:space="preserve">dnabaesjodar@unrn.edu.ar</t>
   </si>
   <si>
@@ -2240,9 +2237,6 @@
     <t xml:space="preserve">lgaribaldi@unrn.edu.ar</t>
   </si>
   <si>
-    <t xml:space="preserve">Consejo Nacional de Investigaciones Cientificas y Tecnicas, Instituto de Investigaciones en Recursos Naturales, Agroecologia y Desarrollo Rural, Rio Negro, Argentina</t>
-  </si>
-  <si>
     <t xml:space="preserve">Eeraerts_etal_sweetcherry_Belgium_2017</t>
   </si>
   <si>
@@ -2261,7 +2255,7 @@
     <t xml:space="preserve">montse.vila@ebd.csic.es</t>
   </si>
   <si>
-    <t xml:space="preserve">Centre Line_Selwyn_Ontario_2017</t>
+    <t xml:space="preserve">Willis_Chan_Raine_Cucurbita_pepo_Canada_2017</t>
   </si>
   <si>
     <t xml:space="preserve">D. Susan Willis Chan</t>
@@ -2270,7 +2264,40 @@
     <t xml:space="preserve">peponapis@yahoo.com </t>
   </si>
   <si>
-    <t xml:space="preserve">Centre Line_Selwyn_Ontario_2018</t>
+    <t xml:space="preserve">Ontario Ministry of Agriculture, Food and Rural Affairs (OMAFRA) Grant UofG2015-2466;
+Ontario Ministry of Environment and Climate Change (MOECC) Best in Science grant
+BIS201617-06; Natural Sciences and Engineering Research Council (NSERC) Discovery
+Grant 2015-06783; Fresh Vegetable Growers of Ontario (FVGO); Food from Thought: Agricultural Systems for a Healthy Planet Initiative, by the Canada First Research
+Excellent Fund (grant 000054)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Willis_Chan_Raine_Cucurbita_pepo_Canada_2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leah_Blechschmidt_Malus_domestica_Canada_2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leah Blechschmidt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lnb.schmidt@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ontario Ministry of Agriculture, Food and Rural Affairs (OMAFRA) Grant UofG2015-2466; 
+Ontario Ministry of Environment and Climate Change (MOECC) Best in Science grant
+BIS201617-06; Natural Sciences and Engineering Research Council (NSERC) Discovery
+Grant 2015-06783; Food from Thought: Agricultural Systems for a Healthy Planet Initiative, by the Canada First Research
+Excellent Fund (grant 000054); W. Garfield Weston Foundation; Natural Sciences and Engineering Research Council Master's level Canada Graduate Scholarship; Ontario Fruit and Vegetable Conference; Ontario Agricultural College at the University of Guelph; University of Guelph; the Arrell Food Institute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ontario Ministry of Agriculture, Food and Rural Affairs (OMAFRA) Grant UofG2015-2466; 
+Ontario Ministry of Environment and Climate Change (MOECC) Best in Science grant
+BIS201617-06; Natural Sciences and Engineering Research Council (NSERC) Discovery
+Grant 2015-06783; Food from Thought: Agricultural Systems for a Healthy Planet Initiative, by the Canada First Research
+Excellent Fund (grant 000054); W. Garfield Weston Foundation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leah_Blechschmidt_Malus_domestica_Canada_2019</t>
   </si>
 </sst>
 </file>
@@ -2280,7 +2307,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2301,6 +2328,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -2431,13 +2465,17 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -2476,7 +2514,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2500,16 +2538,20 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2517,27 +2559,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2545,27 +2587,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2573,7 +2615,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2581,16 +2623,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -2605,11 +2643,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2617,7 +2659,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2625,26 +2667,35 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal 2" xfId="21"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
   </cellStyles>
   <colors>
@@ -2715,18 +2766,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:IW1140"/>
+  <dimension ref="A1:IW1144"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1128" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1137" activeCellId="0" sqref="E1137:E1140"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1103" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1125" activeCellId="0" sqref="F1125"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.40625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="54.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="46.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="40"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="40"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="113.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="44.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="54.98"/>
   </cols>
@@ -30323,69 +30375,69 @@
         <v>729</v>
       </c>
     </row>
-    <row r="1125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1125" customFormat="false" ht="47.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1125" s="0" t="s">
         <v>731</v>
       </c>
       <c r="B1125" s="0" t="s">
         <v>732</v>
       </c>
-      <c r="C1125" s="0" t="s">
+      <c r="C1125" s="10" t="s">
+        <v>640</v>
+      </c>
+      <c r="D1125" s="0" t="s">
         <v>733</v>
-      </c>
-      <c r="D1125" s="0" t="s">
-        <v>734</v>
       </c>
       <c r="E1125" s="0" t="s">
         <v>12</v>
       </c>
       <c r="F1125" s="0" t="s">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="1126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="1126" customFormat="false" ht="47.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1126" s="0" t="s">
         <v>731</v>
       </c>
       <c r="B1126" s="0" t="s">
+        <v>735</v>
+      </c>
+      <c r="C1126" s="10" t="s">
+        <v>640</v>
+      </c>
+      <c r="D1126" s="0" t="s">
         <v>736</v>
       </c>
-      <c r="C1126" s="0" t="s">
-        <v>733</v>
-      </c>
-      <c r="D1126" s="0" t="s">
-        <v>737</v>
-      </c>
       <c r="E1126" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F1126" s="0" t="s">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="1127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="1127" customFormat="false" ht="47.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1127" s="0" t="s">
         <v>731</v>
       </c>
       <c r="B1127" s="0" t="s">
+        <v>735</v>
+      </c>
+      <c r="C1127" s="10" t="s">
+        <v>642</v>
+      </c>
+      <c r="D1127" s="0" t="s">
         <v>736</v>
       </c>
-      <c r="C1127" s="0" t="s">
-        <v>738</v>
-      </c>
-      <c r="D1127" s="0" t="s">
-        <v>737</v>
-      </c>
       <c r="E1127" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F1127" s="0" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="1128" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1128" s="0" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="B1128" s="0" t="s">
         <v>716</v>
@@ -30400,12 +30452,12 @@
         <v>12</v>
       </c>
       <c r="F1128" s="0" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
     </row>
     <row r="1129" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1129" s="0" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="B1129" s="0" t="s">
         <v>722</v>
@@ -30425,7 +30477,7 @@
     </row>
     <row r="1130" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1130" s="0" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="B1130" s="0" t="s">
         <v>720</v>
@@ -30445,7 +30497,7 @@
     </row>
     <row r="1131" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1131" s="0" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="B1131" s="0" t="s">
         <v>716</v>
@@ -30460,12 +30512,12 @@
         <v>12</v>
       </c>
       <c r="F1131" s="0" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
     </row>
     <row r="1132" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1132" s="0" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="B1132" s="0" t="s">
         <v>722</v>
@@ -30485,7 +30537,7 @@
     </row>
     <row r="1133" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1133" s="0" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="B1133" s="0" t="s">
         <v>720</v>
@@ -30505,7 +30557,7 @@
     </row>
     <row r="1134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1134" s="0" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="B1134" s="0" t="s">
         <v>134</v>
@@ -30520,12 +30572,12 @@
         <v>12</v>
       </c>
       <c r="F1134" s="0" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
     </row>
     <row r="1135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1135" s="0" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="B1135" s="0" t="s">
         <v>132</v>
@@ -30545,7 +30597,7 @@
     </row>
     <row r="1136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1136" s="0" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="B1136" s="0" t="s">
         <v>28</v>
@@ -30554,40 +30606,43 @@
         <v>22</v>
       </c>
       <c r="D1136" s="0" t="s">
+        <v>742</v>
+      </c>
+      <c r="E1136" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1136" s="0" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="1137" customFormat="false" ht="72.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1137" s="30" t="s">
+        <v>743</v>
+      </c>
+      <c r="B1137" s="2" t="s">
         <v>744</v>
       </c>
-      <c r="E1136" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1136" s="0" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="1137" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1137" s="30" t="s">
+      <c r="C1137" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1137" s="12" t="s">
         <v>745</v>
       </c>
-      <c r="B1137" s="30" t="s">
+      <c r="E1137" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1137" s="9" t="s">
         <v>746</v>
       </c>
-      <c r="C1137" s="31" t="s">
-        <v>117</v>
-      </c>
-      <c r="D1137" s="32" t="s">
-        <v>747</v>
-      </c>
-      <c r="E1137" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="1138" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="1138" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1138" s="30" t="s">
-        <v>745</v>
-      </c>
-      <c r="B1138" s="30" t="s">
+        <v>743</v>
+      </c>
+      <c r="B1138" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C1138" s="31" t="s">
+      <c r="C1138" s="9" t="s">
         <v>117</v>
       </c>
       <c r="D1138" s="0" t="s">
@@ -30596,32 +30651,38 @@
       <c r="E1138" s="0" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="1139" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1138" s="9" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="1139" customFormat="false" ht="64.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1139" s="30" t="s">
-        <v>748</v>
-      </c>
-      <c r="B1139" s="30" t="s">
+        <v>747</v>
+      </c>
+      <c r="B1139" s="2" t="s">
+        <v>744</v>
+      </c>
+      <c r="C1139" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1139" s="12" t="s">
+        <v>745</v>
+      </c>
+      <c r="E1139" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1139" s="9" t="s">
         <v>746</v>
       </c>
-      <c r="C1139" s="31" t="s">
-        <v>117</v>
-      </c>
-      <c r="D1139" s="32" t="s">
+    </row>
+    <row r="1140" customFormat="false" ht="76.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1140" s="30" t="s">
         <v>747</v>
       </c>
-      <c r="E1139" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="1140" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1140" s="30" t="s">
-        <v>748</v>
-      </c>
-      <c r="B1140" s="30" t="s">
+      <c r="B1140" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C1140" s="31" t="s">
+      <c r="C1140" s="9" t="s">
         <v>117</v>
       </c>
       <c r="D1140" s="0" t="s">
@@ -30629,6 +30690,89 @@
       </c>
       <c r="E1140" s="0" t="s">
         <v>17</v>
+      </c>
+      <c r="F1140" s="9" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="1141" customFormat="false" ht="132.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1141" s="31" t="s">
+        <v>748</v>
+      </c>
+      <c r="B1141" s="31" t="s">
+        <v>749</v>
+      </c>
+      <c r="C1141" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1141" s="32" t="s">
+        <v>750</v>
+      </c>
+      <c r="E1141" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1141" s="33" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="1142" customFormat="false" ht="94.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1142" s="31" t="s">
+        <v>748</v>
+      </c>
+      <c r="B1142" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1142" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1142" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1142" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1142" s="33" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="1143" customFormat="false" ht="83.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1143" s="31" t="s">
+        <v>753</v>
+      </c>
+      <c r="B1143" s="31" t="s">
+        <v>749</v>
+      </c>
+      <c r="C1143" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1143" s="32" t="s">
+        <v>750</v>
+      </c>
+      <c r="E1143" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1143" s="33" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="1144" customFormat="false" ht="92.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1144" s="31" t="s">
+        <v>753</v>
+      </c>
+      <c r="B1144" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1144" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1144" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1144" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1144" s="33" t="s">
+        <v>752</v>
       </c>
     </row>
   </sheetData>
@@ -30705,6 +30849,8 @@
     <hyperlink ref="D1088" r:id="rId70" display="amber.sciligo@gmail.com "/>
     <hyperlink ref="D1110" r:id="rId71" display="fabia714@gmail.com"/>
     <hyperlink ref="D1135" r:id="rId72" display="nacho.bartomeus@gmail.com"/>
+    <hyperlink ref="D1141" r:id="rId73" display="lnb.schmidt@gmail.com"/>
+    <hyperlink ref="D1143" r:id="rId74" display="lnb.schmidt@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Correct study id format in ME_Prunus_Avium_Belgium
</commit_message>
<xml_diff>
--- a/Final_Data/Supporting_files/Verified_studies/FINAL_Data ownership.xlsx
+++ b/Final_Data/Supporting_files/Verified_studies/FINAL_Data ownership.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8306" uniqueCount="754">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8324" uniqueCount="755">
   <si>
     <t xml:space="preserve">study_id</t>
   </si>
@@ -2237,13 +2237,16 @@
     <t xml:space="preserve">lgaribaldi@unrn.edu.ar</t>
   </si>
   <si>
+    <t xml:space="preserve">Eeraerts_etal_sweetcherry_Belgium_2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research Foundation Flanders (FWO) PhD grant 1S71416N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eeraerts_etal_sweetcherry_Belgium_2016</t>
+  </si>
+  <si>
     <t xml:space="preserve">Eeraerts_etal_sweetcherry_Belgium_2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Research Foundation Flanders (FWO) PhD grant 1S71416N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eeraerts_etal_sweetcherry_Belgium_2019</t>
   </si>
   <si>
     <t xml:space="preserve">Carlos_Zaragoza_Trello_Vicia_faba_Ecuador_2017</t>
@@ -2766,13 +2769,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:IW1144"/>
+  <dimension ref="A1:IW1147"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1103" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1125" activeCellId="0" sqref="F1125"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1127" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1133" activeCellId="0" sqref="A1133"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.47265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="54.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.99"/>
@@ -30515,7 +30518,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="1132" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1132" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1132" s="0" t="s">
         <v>739</v>
       </c>
@@ -30535,7 +30538,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1133" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1133" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1133" s="0" t="s">
         <v>739</v>
       </c>
@@ -30555,38 +30558,38 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1134" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1134" s="0" t="s">
         <v>740</v>
       </c>
       <c r="B1134" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="C1134" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1134" s="12" t="s">
-        <v>135</v>
+        <v>716</v>
+      </c>
+      <c r="C1134" s="21" t="s">
+        <v>713</v>
+      </c>
+      <c r="D1134" s="0" t="s">
+        <v>717</v>
       </c>
       <c r="E1134" s="0" t="s">
         <v>12</v>
       </c>
       <c r="F1134" s="0" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="1135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="1135" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1135" s="0" t="s">
         <v>740</v>
       </c>
       <c r="B1135" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="C1135" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1135" s="14" t="s">
-        <v>133</v>
+        <v>722</v>
+      </c>
+      <c r="C1135" s="21" t="s">
+        <v>713</v>
+      </c>
+      <c r="D1135" s="0" t="s">
+        <v>723</v>
       </c>
       <c r="E1135" s="0" t="s">
         <v>17</v>
@@ -30595,184 +30598,244 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1136" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1136" s="0" t="s">
         <v>740</v>
       </c>
       <c r="B1136" s="0" t="s">
+        <v>720</v>
+      </c>
+      <c r="C1136" s="21" t="s">
+        <v>713</v>
+      </c>
+      <c r="D1136" s="0" t="s">
+        <v>721</v>
+      </c>
+      <c r="E1136" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1136" s="0" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="1137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1137" s="0" t="s">
+        <v>741</v>
+      </c>
+      <c r="B1137" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1137" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1137" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1137" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1137" s="0" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="1138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1138" s="0" t="s">
+        <v>741</v>
+      </c>
+      <c r="B1138" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1138" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1138" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="E1138" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1138" s="0" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="1139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1139" s="0" t="s">
+        <v>741</v>
+      </c>
+      <c r="B1139" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C1136" s="4" t="s">
+      <c r="C1139" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D1136" s="0" t="s">
-        <v>742</v>
-      </c>
-      <c r="E1136" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1136" s="0" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="1137" customFormat="false" ht="72.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1137" s="30" t="s">
+      <c r="D1139" s="0" t="s">
         <v>743</v>
       </c>
-      <c r="B1137" s="2" t="s">
+      <c r="E1139" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1139" s="0" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="1140" customFormat="false" ht="72.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1140" s="30" t="s">
         <v>744</v>
       </c>
-      <c r="C1137" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="D1137" s="12" t="s">
+      <c r="B1140" s="2" t="s">
         <v>745</v>
-      </c>
-      <c r="E1137" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1137" s="9" t="s">
-        <v>746</v>
-      </c>
-    </row>
-    <row r="1138" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1138" s="30" t="s">
-        <v>743</v>
-      </c>
-      <c r="B1138" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C1138" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="D1138" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="E1138" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1138" s="9" t="s">
-        <v>746</v>
-      </c>
-    </row>
-    <row r="1139" customFormat="false" ht="64.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1139" s="30" t="s">
-        <v>747</v>
-      </c>
-      <c r="B1139" s="2" t="s">
-        <v>744</v>
-      </c>
-      <c r="C1139" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="D1139" s="12" t="s">
-        <v>745</v>
-      </c>
-      <c r="E1139" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1139" s="9" t="s">
-        <v>746</v>
-      </c>
-    </row>
-    <row r="1140" customFormat="false" ht="76.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1140" s="30" t="s">
-        <v>747</v>
-      </c>
-      <c r="B1140" s="2" t="s">
-        <v>120</v>
       </c>
       <c r="C1140" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="D1140" s="0" t="s">
-        <v>121</v>
+      <c r="D1140" s="12" t="s">
+        <v>746</v>
       </c>
       <c r="E1140" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F1140" s="9" t="s">
-        <v>746</v>
-      </c>
-    </row>
-    <row r="1141" customFormat="false" ht="132.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1141" s="31" t="s">
-        <v>748</v>
-      </c>
-      <c r="B1141" s="31" t="s">
-        <v>749</v>
+        <v>747</v>
+      </c>
+    </row>
+    <row r="1141" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1141" s="30" t="s">
+        <v>744</v>
+      </c>
+      <c r="B1141" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="C1141" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="D1141" s="32" t="s">
-        <v>750</v>
-      </c>
-      <c r="E1141" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1141" s="33" t="s">
-        <v>751</v>
-      </c>
-    </row>
-    <row r="1142" customFormat="false" ht="94.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1142" s="31" t="s">
+      <c r="D1141" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1141" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1141" s="9" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="1142" customFormat="false" ht="64.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1142" s="30" t="s">
         <v>748</v>
       </c>
       <c r="B1142" s="2" t="s">
-        <v>120</v>
+        <v>745</v>
       </c>
       <c r="C1142" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="D1142" s="34" t="s">
-        <v>121</v>
-      </c>
-      <c r="E1142" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1142" s="33" t="s">
-        <v>752</v>
-      </c>
-    </row>
-    <row r="1143" customFormat="false" ht="83.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1143" s="31" t="s">
-        <v>753</v>
-      </c>
-      <c r="B1143" s="31" t="s">
-        <v>749</v>
+      <c r="D1142" s="12" t="s">
+        <v>746</v>
+      </c>
+      <c r="E1142" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1142" s="9" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="1143" customFormat="false" ht="76.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1143" s="30" t="s">
+        <v>748</v>
+      </c>
+      <c r="B1143" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="C1143" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="D1143" s="32" t="s">
+      <c r="D1143" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1143" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1143" s="9" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="1144" customFormat="false" ht="132.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1144" s="31" t="s">
+        <v>749</v>
+      </c>
+      <c r="B1144" s="31" t="s">
         <v>750</v>
-      </c>
-      <c r="E1143" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1143" s="33" t="s">
-        <v>751</v>
-      </c>
-    </row>
-    <row r="1144" customFormat="false" ht="92.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1144" s="31" t="s">
-        <v>753</v>
-      </c>
-      <c r="B1144" s="2" t="s">
-        <v>120</v>
       </c>
       <c r="C1144" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="D1144" s="34" t="s">
-        <v>121</v>
+      <c r="D1144" s="32" t="s">
+        <v>751</v>
       </c>
       <c r="E1144" s="31" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F1144" s="33" t="s">
         <v>752</v>
+      </c>
+    </row>
+    <row r="1145" customFormat="false" ht="94.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1145" s="31" t="s">
+        <v>749</v>
+      </c>
+      <c r="B1145" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1145" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1145" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1145" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1145" s="33" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="1146" customFormat="false" ht="83.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1146" s="31" t="s">
+        <v>754</v>
+      </c>
+      <c r="B1146" s="31" t="s">
+        <v>750</v>
+      </c>
+      <c r="C1146" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1146" s="32" t="s">
+        <v>751</v>
+      </c>
+      <c r="E1146" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1146" s="33" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="1147" customFormat="false" ht="92.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1147" s="31" t="s">
+        <v>754</v>
+      </c>
+      <c r="B1147" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1147" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1147" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1147" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1147" s="33" t="s">
+        <v>753</v>
       </c>
     </row>
   </sheetData>
@@ -30848,9 +30911,9 @@
     <hyperlink ref="D1083" r:id="rId69" display="riastewart30@gmail.com "/>
     <hyperlink ref="D1088" r:id="rId70" display="amber.sciligo@gmail.com "/>
     <hyperlink ref="D1110" r:id="rId71" display="fabia714@gmail.com"/>
-    <hyperlink ref="D1135" r:id="rId72" display="nacho.bartomeus@gmail.com"/>
-    <hyperlink ref="D1141" r:id="rId73" display="lnb.schmidt@gmail.com"/>
-    <hyperlink ref="D1143" r:id="rId74" display="lnb.schmidt@gmail.com"/>
+    <hyperlink ref="D1138" r:id="rId72" display="nacho.bartomeus@gmail.com"/>
+    <hyperlink ref="D1144" r:id="rId73" display="lnb.schmidt@gmail.com"/>
+    <hyperlink ref="D1146" r:id="rId74" display="lnb.schmidt@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>